<commit_message>
QA updates to Profiles inlcuding applying GF#19908 to diagnosticreport and Lab Observation
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-server.xlsx
+++ b/source/source_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF9079E-9413-1944-87BB-99322474FCD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2309E4D3-70CC-4F3F-BD59-443099C170E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -817,12 +816,6 @@
     <t>reference,token,date</t>
   </si>
   <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://hl7.org/fhir/observation-category\|laboratory</t>
-  </si>
-  <si>
-    <t>GET [base]Observation?patient=555580&amp;category=http://hl7.org/fhir/observation-category\|laboratory&amp;date=ge2018-03-14</t>
-  </si>
-  <si>
     <t>patient,code,date</t>
   </si>
   <si>
@@ -1051,15 +1044,6 @@
     <t>support searching for all laboratory results for a patient for a given status (for example all observations marked as final)</t>
   </si>
   <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://hl7.org/fhir/observation-category\|laboratory&amp;status=final</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://hl7.org/fhir/observation-category\|vital-signs</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://hl7.org/fhir/observation-category\|vital-signs&amp;status=final</t>
-  </si>
-  <si>
     <t>support searching for all vital sign observations by code (for example, search for all heart rate, respiratory rate and blood pressure observations for a patient)</t>
   </si>
   <si>
@@ -1069,9 +1053,6 @@
     <t>GET [base]/Observation?patient=1186747&amp;code=http://loinc.org\|8867-4,http://loinc.org\|9279-1,http://loinc.org\|85354-9&amp;date=ge2019</t>
   </si>
   <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://hl7.org/fhir/observation-category\|vital-signs&amp;date=ge2019</t>
-  </si>
-  <si>
     <t>support searching for all vital sign observations by date (for example, find all the vital sign observations for 2019)</t>
   </si>
   <si>
@@ -1216,16 +1197,10 @@
     <t>category=http://terminology.hl7.org/CodeSystem/v2-0074|LAB</t>
   </si>
   <si>
-    <t>category=http://hl7.org/fhir/observation-category|laboratory</t>
-  </si>
-  <si>
     <t>category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category|assess-plan</t>
   </si>
   <si>
     <t>code=http://loinc.org|72166-2</t>
-  </si>
-  <si>
-    <t>category=http://hl7.org/fhir/observation-category|vital-signs</t>
   </si>
   <si>
     <t>category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category|clinical-note</t>
@@ -1598,12 +1573,36 @@
     <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
 `GET [base]/DocumentReference/$docref?patient=[id]`</t>
   </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|laboratory</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;status=final</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;date=ge2018-03-14</t>
+  </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|vital-signs</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;status=final</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;date=ge2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2069,13 +2068,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2083,31 +2082,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105" customHeight="1">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2115,20 +2114,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="351.75" customHeight="1">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="103.5" customHeight="1">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -2144,9 +2143,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2167,15 +2166,15 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2189,27 +2188,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2219,42 +2218,42 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2264,12 +2263,12 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -2279,12 +2278,12 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -2294,12 +2293,12 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -2309,12 +2308,12 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -2324,12 +2323,12 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -2339,12 +2338,12 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -2354,27 +2353,27 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -2384,12 +2383,12 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -2399,27 +2398,27 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -2429,12 +2428,12 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -2444,42 +2443,42 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
@@ -2489,27 +2488,27 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="11" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -2519,12 +2518,12 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
@@ -2534,12 +2533,12 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
@@ -2566,22 +2565,22 @@
       <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
-    <col min="20" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="18" thickBot="1">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2595,67 +2594,67 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="X1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="38.25" customHeight="1" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2675,9 +2674,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -2689,9 +2688,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -2703,7 +2702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
         <v>148</v>
       </c>
@@ -2720,9 +2719,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -2734,7 +2733,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" s="1" t="s">
         <v>192</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="75">
       <c r="A8" s="1" t="s">
         <v>191</v>
       </c>
@@ -2756,7 +2755,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>21</v>
@@ -2765,7 +2764,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" s="1" t="s">
         <v>193</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
         <v>172</v>
       </c>
@@ -2807,9 +2806,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
@@ -2821,15 +2820,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="105">
       <c r="A13" s="1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>21</v>
@@ -2838,7 +2837,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="288" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="315">
       <c r="A14" s="1" t="s">
         <v>194</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>21</v>
@@ -2858,7 +2857,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="288" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="315">
       <c r="A15" s="1" t="s">
         <v>197</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>21</v>
@@ -2875,10 +2874,10 @@
         <v>78</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="1" t="s">
         <v>196</v>
       </c>
@@ -2892,9 +2891,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -2906,7 +2905,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -2920,9 +2919,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21">
       <c r="A19" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -2934,9 +2933,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21">
       <c r="A20" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -2948,10 +2947,10 @@
         <v>78</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>195</v>
       </c>
@@ -2965,28 +2964,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21">
       <c r="A25"/>
     </row>
-    <row r="56" spans="20:23" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="20:23" ht="18">
       <c r="T56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
     </row>
-    <row r="59" spans="20:23" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="20:23" ht="18">
       <c r="W59" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
+  <sortState ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3003,15 +3002,15 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -3028,12 +3027,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="135.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>191</v>
@@ -3042,10 +3041,10 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -3057,84 +3056,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3394,7 +3393,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3459,7 +3458,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -3524,7 +3523,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3732,37 +3731,37 @@
       <pane xSplit="6" ySplit="1" topLeftCell="AA41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB54" sqref="AB54"/>
+      <selection pane="bottomRight" activeCell="AB62" sqref="AB62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" customWidth="1"/>
+    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -3824,10 +3823,10 @@
         <v>56</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>57</v>
@@ -3848,7 +3847,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3945,7 +3944,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3999,7 +3998,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4058,12 +4057,12 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>68</v>
@@ -4108,7 +4107,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="18.95" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="18.95" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4208,7 +4207,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="18.95" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4254,7 +4253,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="18.95" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4313,7 +4312,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="18.95" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="18.95" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4412,7 +4411,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="18.95" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="18.95" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>227</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="AA14" s="2" t="s">
         <v>183</v>
@@ -4523,7 +4522,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4573,7 +4572,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="18.95" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4627,7 +4626,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="18.95" customHeight="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="18.95" customHeight="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4739,7 +4738,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="18.95" customHeight="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4789,7 +4788,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="18.95" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="18.95" customHeight="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4880,14 +4879,14 @@
         <v>84</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="AB21" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;SUBSTITUTE(C21,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="18.95" customHeight="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4938,7 +4937,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="18.95" customHeight="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4982,7 +4981,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="18.95" customHeight="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="18.95" customHeight="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="18.95" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5130,7 +5129,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="18.95" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5188,7 +5187,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="18.95" customHeight="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5231,7 +5230,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="18.95" customHeight="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5276,7 +5275,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="18.95" customHeight="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5326,7 +5325,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="18.95" customHeight="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5373,7 +5372,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5433,7 +5432,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5478,7 +5477,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5523,7 +5522,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5574,7 +5573,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5621,7 +5620,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5680,7 +5679,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5784,7 +5783,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5824,20 +5823,20 @@
         <v>62</v>
       </c>
       <c r="Y40" s="5" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="Z40" s="5" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="AA40" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="AB40" s="1" t="str">
         <f t="shared" ref="AB40" si="13">"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5887,7 +5886,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5946,7 +5945,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5996,7 +5995,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6043,7 +6042,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6097,7 +6096,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6105,7 +6104,7 @@
         <v>191</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>34</v>
@@ -6127,7 +6126,7 @@
         <v>88</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>62</v>
@@ -6150,7 +6149,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6200,7 +6199,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6259,7 +6258,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6359,7 +6358,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6413,7 +6412,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6421,7 +6420,7 @@
         <v>193</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>34</v>
@@ -6463,7 +6462,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6522,7 +6521,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6530,7 +6529,7 @@
         <v>193</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>34</v>
@@ -6576,7 +6575,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6626,7 +6625,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6676,7 +6675,7 @@
         <v>230</v>
       </c>
       <c r="Z56" s="12" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="AA56" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -6687,7 +6686,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6695,7 +6694,7 @@
         <v>194</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>34</v>
@@ -6741,7 +6740,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6791,7 +6790,7 @@
         <v>SearchParameter-us-core-medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6831,7 +6830,7 @@
         <v>62</v>
       </c>
       <c r="V59" s="7" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="X59" s="1" t="s">
         <v>101</v>
@@ -6840,7 +6839,7 @@
         <v>231</v>
       </c>
       <c r="Z59" s="12" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="AA59" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B59&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -6851,7 +6850,7 @@
         <v>SearchParameter-us-core-medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -6859,7 +6858,7 @@
         <v>197</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>34</v>
@@ -6905,7 +6904,7 @@
         <v>SearchParameter-us-core-medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7013,7 +7012,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7067,7 +7066,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7117,7 +7116,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7167,7 +7166,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7217,7 +7216,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7267,7 +7266,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7321,7 +7320,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7380,12 +7379,12 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>150</v>
@@ -7430,12 +7429,12 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>30</v>
@@ -7477,12 +7476,12 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>88</v>
@@ -7531,12 +7530,12 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>99</v>
@@ -7590,12 +7589,12 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>68</v>
@@ -7640,12 +7639,12 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>99</v>
@@ -7699,12 +7698,12 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>68</v>
@@ -7749,12 +7748,12 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>99</v>
@@ -7808,12 +7807,12 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>14</v>
@@ -7854,12 +7853,12 @@
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="18.95" customHeight="1">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>27</v>
@@ -7894,10 +7893,10 @@
         <v>62</v>
       </c>
       <c r="Y79" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Z79" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AA79" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp; " resources that match the name"</f>
@@ -7908,12 +7907,12 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="18.95" customHeight="1">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>95</v>
@@ -7948,10 +7947,10 @@
         <v>62</v>
       </c>
       <c r="Y80" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Z80" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AA80" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp; " resources that match the address string"</f>
@@ -7962,15 +7961,15 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="18.95" customHeight="1">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>78</v>
@@ -8002,10 +8001,10 @@
         <v>62</v>
       </c>
       <c r="Y81" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Z81" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AA81" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp; " resources for the city"</f>
@@ -8016,15 +8015,15 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="18.95" customHeight="1">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>78</v>
@@ -8056,10 +8055,10 @@
         <v>62</v>
       </c>
       <c r="Y82" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="Z82" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AA82" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp; " resources for the state"</f>
@@ -8070,15 +8069,15 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="18.95" customHeight="1">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>78</v>
@@ -8110,10 +8109,10 @@
         <v>62</v>
       </c>
       <c r="Y83" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="Z83" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AA83" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp; " resources for the ZIP code"</f>
@@ -8124,12 +8123,12 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>27</v>
@@ -8164,10 +8163,10 @@
         <v>62</v>
       </c>
       <c r="Y84" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Z84" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AA84" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources that match the name"</f>
@@ -8178,12 +8177,12 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>95</v>
@@ -8218,10 +8217,10 @@
         <v>62</v>
       </c>
       <c r="Y85" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Z85" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AA85" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp; " resources that match the address string"</f>
@@ -8232,15 +8231,15 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>78</v>
@@ -8272,10 +8271,10 @@
         <v>62</v>
       </c>
       <c r="Y86" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Z86" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AA86" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp; " resources for the city"</f>
@@ -8286,15 +8285,15 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>78</v>
@@ -8326,10 +8325,10 @@
         <v>62</v>
       </c>
       <c r="Y87" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Z87" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AA87" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp; " resources for the state"</f>
@@ -8340,15 +8339,15 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>78</v>
@@ -8380,10 +8379,10 @@
         <v>62</v>
       </c>
       <c r="Y88" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Z88" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AA88" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp; " resources for the ZIP code"</f>
@@ -8394,12 +8393,12 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>27</v>
@@ -8437,10 +8436,10 @@
         <v>86</v>
       </c>
       <c r="Y89" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="Z89" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AA89" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources matching the name"</f>
@@ -8451,12 +8450,12 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>85</v>
@@ -8491,10 +8490,10 @@
         <v>62</v>
       </c>
       <c r="Y90" s="5" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="Z90" s="7" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="AA90" s="12" t="str">
         <f>"Fetches a bundle containing any "&amp;B90&amp;" resources matching the identifier"</f>
@@ -8505,15 +8504,15 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>13</v>
@@ -8545,13 +8544,13 @@
         <v>62</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="Y91" s="5" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="Z91" s="7" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="AA91" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B91&amp;" resources matching the specialty"</f>
@@ -8562,15 +8561,15 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="18.95" customHeight="1">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>13</v>
@@ -8602,16 +8601,16 @@
         <v>62</v>
       </c>
       <c r="S92" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="V92" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y92" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="V92" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="Y92" s="5" t="s">
-        <v>307</v>
-      </c>
       <c r="Z92" s="7" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="AA92" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B92&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
@@ -8622,12 +8621,12 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="18.95" customHeight="1">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
+  <sortState ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8640,28 +8639,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomRight" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
@@ -8681,7 +8680,7 @@
         <v>108</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -8693,7 +8692,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8718,7 +8717,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -8743,7 +8742,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -8768,7 +8767,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -8793,7 +8792,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -8814,17 +8813,17 @@
         <v>116</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="J6" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -8849,7 +8848,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -8874,7 +8873,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -8900,7 +8899,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -8927,7 +8926,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -8953,7 +8952,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -8978,7 +8977,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -8999,17 +8998,17 @@
         <v>123</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="J13" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9034,7 +9033,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9059,7 +9058,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9080,17 +9079,17 @@
         <v>116</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="J16" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9116,7 +9115,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9137,17 +9136,17 @@
         <v>116</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="J18" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -9200,7 +9199,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -9225,7 +9224,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9251,7 +9250,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9278,7 +9277,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9305,7 +9304,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9332,7 +9331,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9357,7 +9356,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9382,7 +9381,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9407,7 +9406,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -9438,7 +9437,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -9469,7 +9468,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -9500,7 +9499,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -9531,7 +9530,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -9552,19 +9551,19 @@
         <v>116</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>166</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -9588,13 +9587,13 @@
         <v>160</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -9618,13 +9617,13 @@
         <v>161</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="1" customFormat="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -9654,7 +9653,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -9678,13 +9677,13 @@
         <v>173</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="1" customFormat="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -9715,7 +9714,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="1" customFormat="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -9736,7 +9735,7 @@
         <v>159</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>174</v>
@@ -9746,7 +9745,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="1" customFormat="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -9776,7 +9775,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -9796,7 +9795,7 @@
         <v>116</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>207</v>
@@ -9809,7 +9808,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -9829,7 +9828,7 @@
         <v>116</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>212</v>
@@ -9839,7 +9838,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -9859,7 +9858,7 @@
         <v>235</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>209</v>
@@ -9872,7 +9871,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" s="1" customFormat="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -9883,7 +9882,7 @@
         <v>202</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>78</v>
@@ -9892,17 +9891,17 @@
         <v>235</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="1" customFormat="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -9922,7 +9921,7 @@
         <v>116</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>198</v>
@@ -9932,7 +9931,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" s="1" customFormat="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -9962,7 +9961,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" s="1" customFormat="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -9992,7 +9991,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="1" customFormat="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -10022,7 +10021,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" s="1" customFormat="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -10033,7 +10032,7 @@
         <v>203</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>78</v>
@@ -10042,17 +10041,17 @@
         <v>235</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" s="1" customFormat="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -10064,7 +10063,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>78</v>
@@ -10076,14 +10075,14 @@
         <v>200</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="J50" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" s="1" customFormat="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -10095,7 +10094,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>78</v>
@@ -10107,14 +10106,14 @@
         <v>223</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="J51" s="5" t="str">
         <f t="shared" ref="J51" si="6">"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="1" customFormat="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -10138,13 +10137,13 @@
         <v>199</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="1" customFormat="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -10156,7 +10155,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>78</v>
@@ -10165,16 +10164,16 @@
         <v>159</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="1" customFormat="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -10198,14 +10197,14 @@
         <v>201</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="J54" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Fetches a bundle of all MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" s="1" customFormat="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -10217,7 +10216,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>78</v>
@@ -10226,16 +10225,16 @@
         <v>159</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="1" customFormat="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10266,7 +10265,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" s="1" customFormat="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10297,7 +10296,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" s="1" customFormat="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10309,7 +10308,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>78</v>
@@ -10318,17 +10317,17 @@
         <v>235</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J58" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B58&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" s="1" customFormat="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -10336,10 +10335,10 @@
         <v>196</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>78</v>
@@ -10348,19 +10347,19 @@
         <v>116</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>369</v>
+        <v>482</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>314</v>
+        <v>483</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="1" customFormat="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -10368,7 +10367,7 @@
         <v>196</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>155</v>
@@ -10380,20 +10379,20 @@
         <v>116</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>369</v>
+        <v>482</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>236</v>
+        <v>484</v>
       </c>
       <c r="J60" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B60&amp;" resources for the specified patient and a category code = `laboratory`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" s="1" customFormat="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -10401,7 +10400,7 @@
         <v>196</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>157</v>
@@ -10413,17 +10412,17 @@
         <v>116</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J61" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B61&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" s="1" customFormat="1">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -10431,7 +10430,7 @@
         <v>196</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>208</v>
@@ -10443,20 +10442,20 @@
         <v>235</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>369</v>
+        <v>482</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>237</v>
+        <v>485</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" s="1" customFormat="1">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -10464,10 +10463,10 @@
         <v>196</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>78</v>
@@ -10476,25 +10475,25 @@
         <v>235</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J63" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B63&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" s="1" customFormat="1">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>126</v>
@@ -10516,15 +10515,15 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" s="1" customFormat="1">
       <c r="A65" s="1">
         <v>58</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65" s="11" t="s">
         <v>259</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>155</v>
@@ -10536,28 +10535,28 @@
         <v>116</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J65" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")&amp;"=`assess-plan`"</f>
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" s="1" customFormat="1">
       <c r="A66" s="1">
         <v>59</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>259</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>208</v>
@@ -10569,30 +10568,30 @@
         <v>235</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" s="1" customFormat="1">
       <c r="A67" s="1">
         <v>61</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="C67" s="11" t="s">
-        <v>261</v>
-      </c>
       <c r="D67" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>78</v>
@@ -10601,30 +10600,30 @@
         <v>116</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I67" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="J67" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="J67" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:16" s="1" customFormat="1">
       <c r="A68" s="1">
         <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="D68" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>78</v>
@@ -10633,24 +10632,24 @@
         <v>235</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" s="1" customFormat="1">
       <c r="A69" s="1">
         <v>63</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" ref="C69" si="9">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B69)</f>
@@ -10666,19 +10665,19 @@
         <v>116</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="H69" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="J69" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="I69" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:16" ht="15.75">
       <c r="A70" s="1">
         <v>64</v>
       </c>
@@ -10686,7 +10685,7 @@
         <v>196</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>157</v>
@@ -10698,13 +10697,13 @@
         <v>116</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J70" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and observation code."</f>
@@ -10717,7 +10716,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" s="1" customFormat="1">
       <c r="A71" s="1">
         <v>58</v>
       </c>
@@ -10725,10 +10724,10 @@
         <v>196</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>78</v>
@@ -10737,20 +10736,20 @@
         <v>116</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>372</v>
+        <v>486</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>316</v>
+        <v>487</v>
       </c>
       <c r="J71" s="5" t="str">
         <f t="shared" ref="J71" si="10">"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ")</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" s="1" customFormat="1">
       <c r="A72" s="1">
         <v>59</v>
       </c>
@@ -10758,7 +10757,7 @@
         <v>196</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>155</v>
@@ -10770,20 +10769,20 @@
         <v>116</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>372</v>
+        <v>486</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>315</v>
+        <v>488</v>
       </c>
       <c r="J72" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" s="1" customFormat="1">
       <c r="A73" s="1">
         <v>60</v>
       </c>
@@ -10791,7 +10790,7 @@
         <v>196</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>157</v>
@@ -10803,20 +10802,20 @@
         <v>116</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>372</v>
+        <v>486</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only."</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" s="1" customFormat="1">
       <c r="A74" s="1">
         <v>61</v>
       </c>
@@ -10824,7 +10823,7 @@
         <v>196</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>208</v>
@@ -10836,20 +10835,20 @@
         <v>235</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>372</v>
+        <v>486</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="1" customFormat="1">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -10857,10 +10856,10 @@
         <v>196</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>78</v>
@@ -10869,17 +10868,17 @@
         <v>235</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="J75" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B75&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="1" customFormat="1">
       <c r="A76" s="1">
         <v>39</v>
       </c>
@@ -10900,29 +10899,29 @@
         <v>116</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified "&amp;SUBSTITUTE(D76,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="1" customFormat="1">
       <c r="A77" s="1">
         <v>43</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C77" s="1" t="str">
         <f t="shared" ref="C77" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>78</v>
@@ -10931,7 +10930,7 @@
         <v>159</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5" t="str">
@@ -10939,7 +10938,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="1" customFormat="1">
       <c r="A78" s="1">
         <v>40</v>
       </c>
@@ -10960,19 +10959,19 @@
         <v>116</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
       <c r="A79" s="1">
         <v>42</v>
       </c>
@@ -10993,19 +10992,19 @@
         <v>235</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" s="1" customFormat="1">
       <c r="A80" s="1">
         <v>41</v>
       </c>
@@ -11026,16 +11025,16 @@
         <v>116</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="1" customFormat="1">
       <c r="A81" s="1">
         <v>43</v>
       </c>
@@ -11047,7 +11046,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>78</v>
@@ -11056,22 +11055,22 @@
         <v>235</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="J81" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp;" resources for the specified "&amp;SUBSTITUTE(D81,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" s="1" customFormat="1">
       <c r="A82" s="1">
         <v>41</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C82" s="1" t="str">
         <f t="shared" ref="C82" si="13">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
@@ -11087,13 +11086,13 @@
         <v>116</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix CapStatement QA Errors, UPdate US Core Vaccine National Drug Codes (NDC) to most recent CDC update
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-server.xlsx
+++ b/source/source_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D754309-2217-4EC7-AF61-EF4D0ACD8CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A17806C-4325-4298-945F-6A65C35E0781}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="492">
   <si>
     <t>Element</t>
   </si>
@@ -1482,120 +1482,126 @@
     <t>The MedicationStatement and MedicationRequest resources can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationStatement or a MedicationRequest, then the READ and SEARCH Criteria  **SHALL**  be supported.</t>
   </si>
   <si>
-    <t xml:space="preserve"> The MedicationStatement resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+    <t>us-core-server</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.r4-4.0.0</t>
+  </si>
+  <si>
+    <t>versioning_conf</t>
+  </si>
+  <si>
+    <t>readHistory_conf</t>
+  </si>
+  <si>
+    <t>updateCreate_conf</t>
+  </si>
+  <si>
+    <t>conditionalCreate_conf</t>
+  </si>
+  <si>
+    <t>conditionalRead_conf</t>
+  </si>
+  <si>
+    <t>conditionalUpdate_conf</t>
+  </si>
+  <si>
+    <t>conditionalDelete_conf</t>
+  </si>
+  <si>
+    <t>referencePolicy_conf</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;status=active&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=1137192&amp;status=active~GET [base]/MedicationStatement?patient=1137192&amp;status=active&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;effective=ge2019~GET [base]/MedicationStatement?patient=1137192&amp;effective=ge2019&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=1137192&amp;date=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;date=ge2019&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>target-date</t>
+  </si>
+  <si>
+    <t>patient,target-date</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;target-date=ge2015-01-14&amp;target-date=le2019-01-14</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2018&amp;date=le2018</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018&amp;date=le2019</t>
+  </si>
+  <si>
+    <t>The DocumentReference.type binding SHALL support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set</t>
+  </si>
+  <si>
+    <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.
+1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
+  </si>
+  <si>
+    <t>US Core Laboratory Result Observation Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-lab</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height</t>
+  </si>
+  <si>
+    <t>US Core Pediatric BMI for Age Observation Profile</t>
+  </si>
+  <si>
+    <t>US Core Pediatric Weight  for Height Observation Profile</t>
+  </si>
+  <si>
+    <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
+`GET [base]/DocumentReference/$docref?patient=[id]`</t>
+  </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|laboratory</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;status=final</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;date=ge2018-03-14</t>
+  </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|vital-signs</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;status=final</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;date=ge2019</t>
+  </si>
+  <si>
+    <t>doc_DiagnosticReport</t>
+  </si>
+  <si>
+    <t>This conformance expectation applies **only**  to the *US Core DiagnosticReport Profile for Report and Note exchange* profile.  The conformance expectation for the *US Core DiagnosticReport Profile for Laboratory Results Reporting* is  **MAY**.</t>
+  </si>
+  <si>
+    <t>The MedicationStatement resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
  For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
  `GET /MedicationStatement?patient=[id]`
  `GET /MedicationStatement?patient=[id]&amp;_include=MedicationStatement:medication`</t>
-  </si>
-  <si>
-    <t>us-core-server</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.r4-4.0.0</t>
-  </si>
-  <si>
-    <t>versioning_conf</t>
-  </si>
-  <si>
-    <t>readHistory_conf</t>
-  </si>
-  <si>
-    <t>updateCreate_conf</t>
-  </si>
-  <si>
-    <t>conditionalCreate_conf</t>
-  </si>
-  <si>
-    <t>conditionalRead_conf</t>
-  </si>
-  <si>
-    <t>conditionalUpdate_conf</t>
-  </si>
-  <si>
-    <t>conditionalDelete_conf</t>
-  </si>
-  <si>
-    <t>referencePolicy_conf</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;status=active&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationStatement?patient=1137192&amp;status=active~GET [base]/MedicationStatement?patient=1137192&amp;status=active&amp;_include=MedicationStatement:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;effective=ge2019~GET [base]/MedicationStatement?patient=1137192&amp;effective=ge2019&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationStatement?patient=1137192&amp;date=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;date=ge2019&amp;_include=MedicationStatement:medication</t>
-  </si>
-  <si>
-    <t>target-date</t>
-  </si>
-  <si>
-    <t>patient,target-date</t>
-  </si>
-  <si>
-    <t>GET [base]/Goal?patient=1137192&amp;target-date=ge2015-01-14&amp;target-date=le2019-01-14</t>
-  </si>
-  <si>
-    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2018&amp;date=le2018</t>
-  </si>
-  <si>
-    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018&amp;date=le2019</t>
-  </si>
-  <si>
-    <t>The DocumentReference.type binding SHALL support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set</t>
-  </si>
-  <si>
-    <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.
-1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
-  </si>
-  <si>
-    <t>US Core Laboratory Result Observation Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-lab</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-bmi-for-age</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/pediatric-weight-for-height</t>
-  </si>
-  <si>
-    <t>US Core Pediatric BMI for Age Observation Profile</t>
-  </si>
-  <si>
-    <t>US Core Pediatric Weight  for Height Observation Profile</t>
-  </si>
-  <si>
-    <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
-`GET [base]/DocumentReference/$docref?patient=[id]`</t>
-  </si>
-  <si>
-    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|laboratory</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;status=final</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory</t>
-  </si>
-  <si>
-    <t>GET [base]Observation?patient=555580&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|laboratory&amp;date=ge2018-03-14</t>
-  </si>
-  <si>
-    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|vital-signs</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;status=final</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=1134281&amp;category=http://terminology.hl7.org/CodeSystem/observation-category\|vital-signs&amp;date=ge2019</t>
   </si>
 </sst>
 </file>
@@ -2087,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" customHeight="1">
@@ -2103,7 +2109,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2127,7 +2133,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -2370,10 +2376,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -2415,10 +2421,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -2505,10 +2511,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -2558,11 +2564,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2594,49 +2600,49 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>444</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>445</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>449</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>450</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>352</v>
@@ -2755,7 +2761,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>21</v>
@@ -2845,7 +2851,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>453</v>
+        <v>491</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>21</v>
@@ -2865,7 +2871,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>453</v>
+        <v>491</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>21</v>
@@ -3041,7 +3047,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3054,10 +3060,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3065,10 +3071,11 @@
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3087,53 +3094,56 @@
       <c r="F1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22" ht="75">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3152,14 +3162,14 @@
       <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
-        <v>34</v>
+      <c r="G2" s="2" t="s">
+        <v>490</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
         <v>34</v>
@@ -3197,8 +3207,11 @@
       <c r="U2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3217,9 +3230,6 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
@@ -3262,8 +3272,11 @@
       <c r="U3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3282,9 +3295,6 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
@@ -3327,8 +3337,11 @@
       <c r="U4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3347,9 +3360,6 @@
       <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" t="s">
-        <v>78</v>
-      </c>
       <c r="H5" t="s">
         <v>78</v>
       </c>
@@ -3392,8 +3402,11 @@
       <c r="U5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3412,9 +3425,6 @@
       <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
@@ -3457,8 +3467,11 @@
       <c r="U6" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -3477,9 +3490,6 @@
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
@@ -3522,8 +3532,11 @@
       <c r="U7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3542,9 +3555,6 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
       <c r="H8" t="s">
         <v>34</v>
       </c>
@@ -3587,8 +3597,11 @@
       <c r="U8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="V8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3607,9 +3620,6 @@
       <c r="F9" t="s">
         <v>78</v>
       </c>
-      <c r="G9" t="s">
-        <v>78</v>
-      </c>
       <c r="H9" t="s">
         <v>78</v>
       </c>
@@ -3652,8 +3662,11 @@
       <c r="U9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3672,9 +3685,6 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" t="s">
-        <v>34</v>
-      </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
@@ -3715,6 +3725,9 @@
         <v>34</v>
       </c>
       <c r="U10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3727,7 +3740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6526,7 +6539,7 @@
         <v>193</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>34</v>
@@ -10091,7 +10104,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>78</v>
@@ -10103,7 +10116,7 @@
         <v>223</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J51" s="5" t="str">
         <f t="shared" ref="J51" si="6">"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
@@ -10134,7 +10147,7 @@
         <v>199</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>254</v>
@@ -10164,7 +10177,7 @@
         <v>250</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>255</v>
@@ -10194,7 +10207,7 @@
         <v>201</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J54" s="5" t="str">
         <f t="shared" si="4"/>
@@ -10225,7 +10238,7 @@
         <v>251</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>256</v>
@@ -10332,7 +10345,7 @@
         <v>196</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>260</v>
@@ -10344,13 +10357,13 @@
         <v>116</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>311</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J59" s="5" t="s">
         <v>356</v>
@@ -10364,7 +10377,7 @@
         <v>196</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>155</v>
@@ -10376,13 +10389,13 @@
         <v>116</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>239</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J60" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B60&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -10397,7 +10410,7 @@
         <v>196</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>157</v>
@@ -10427,7 +10440,7 @@
         <v>196</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>208</v>
@@ -10439,13 +10452,13 @@
         <v>235</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>244</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -10460,7 +10473,7 @@
         <v>196</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>236</v>
@@ -10490,7 +10503,7 @@
         <v>355</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>126</v>
@@ -10571,7 +10584,7 @@
         <v>264</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>268</v>
@@ -10635,7 +10648,7 @@
         <v>263</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>270</v>
@@ -10733,13 +10746,13 @@
         <v>116</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>310</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J71" s="5" t="str">
         <f t="shared" ref="J71" si="10">"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ")</f>
@@ -10766,13 +10779,13 @@
         <v>116</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>309</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J72" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -10799,7 +10812,7 @@
         <v>116</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>312</v>
@@ -10832,13 +10845,13 @@
         <v>235</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>315</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>

</xml_diff>

<commit_message>
add Should to multipleOrs for Patient and refer to guidance on multiple patients. fixed some bad links
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-server.xlsx
+++ b/source/source_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA686D4-CFEF-4B7F-A1B3-4C5D0B2C4F09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967313B3-02C2-4036-ADA6-66FD343E9D06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="516">
   <si>
     <t>Element</t>
   </si>
@@ -4052,11 +4052,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB95"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="AA65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="AA80" sqref="AA80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
@@ -4359,6 +4359,9 @@
       <c r="K5" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L5" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M5" s="1" t="s">
         <v>62</v>
       </c>
@@ -4616,6 +4619,9 @@
       </c>
       <c r="K10" s="1" t="s">
         <v>62</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>62</v>
@@ -4776,6 +4782,9 @@
       <c r="K13" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L13" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M13" s="1" t="s">
         <v>62</v>
       </c>
@@ -5044,6 +5053,9 @@
       </c>
       <c r="K18" s="1" t="s">
         <v>62</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>62</v>
@@ -5982,6 +5994,9 @@
       <c r="K37" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L37" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M37" s="1" t="s">
         <v>62</v>
       </c>
@@ -6251,6 +6266,9 @@
       <c r="K42" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L42" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M42" s="1" t="s">
         <v>62</v>
       </c>
@@ -6567,6 +6585,9 @@
       <c r="K48" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L48" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M48" s="1" t="s">
         <v>62</v>
       </c>
@@ -6830,6 +6851,9 @@
       <c r="K53" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L53" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M53" s="1" t="s">
         <v>62</v>
       </c>
@@ -7046,6 +7070,9 @@
       <c r="K57" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L57" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M57" s="1" t="s">
         <v>62</v>
       </c>
@@ -7255,6 +7282,9 @@
       <c r="K61" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L61" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M61" s="1" t="s">
         <v>62</v>
       </c>
@@ -7420,6 +7450,9 @@
       <c r="K64" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L64" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M64" s="1" t="s">
         <v>62</v>
       </c>
@@ -7789,6 +7822,9 @@
       <c r="K71" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L71" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M71" s="1" t="s">
         <v>62</v>
       </c>
@@ -7999,6 +8035,9 @@
       <c r="K75" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L75" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M75" s="1" t="s">
         <v>62</v>
       </c>
@@ -8111,6 +8150,9 @@
       <c r="K77" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L77" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M77" s="1" t="s">
         <v>62</v>
       </c>
@@ -8204,8 +8246,8 @@
         <v>1</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f t="shared" si="29"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B79)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-device</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>62</v>
@@ -8223,6 +8265,9 @@
       <c r="K79" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="L79" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="M79" s="1" t="s">
         <v>62</v>
       </c>
@@ -8263,8 +8308,8 @@
         <v>0</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f t="shared" si="29"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B80)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-device</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>62</v>
@@ -9078,11 +9123,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G56" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomRight" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
remove multipleOr for patient parameter, revinclude for Provenance, edited Provenance and =quick start, DocumentReference Quick Start,edits to multiplePatient, added TimeZone section, GF#23735, GF#23734
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-server.xlsx
+++ b/source/source_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2713329-AFD3-4663-A8A9-41EDF2988C08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025AA6C0-E1F3-4EE6-8E06-FE0D9768B58F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -141,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="515">
   <si>
     <t>Element</t>
   </si>
@@ -1694,9 +1695,6 @@
   </si>
   <si>
     <t>If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.</t>
-  </si>
-  <si>
-    <t>Provenance:target</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-provenance</t>
@@ -2279,7 +2277,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2636,10 +2634,10 @@
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
       <c r="A24" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
@@ -2680,10 +2678,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>512</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -2704,10 +2702,10 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2815,9 +2813,6 @@
       <c r="S2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>510</v>
-      </c>
       <c r="X2" t="s">
         <v>22</v>
       </c>
@@ -2835,9 +2830,6 @@
       <c r="S3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
@@ -2852,9 +2844,6 @@
       <c r="S4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
@@ -2869,9 +2858,6 @@
       <c r="S5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>510</v>
-      </c>
       <c r="X5" t="s">
         <v>26</v>
       </c>
@@ -2889,9 +2875,6 @@
       <c r="S6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="1" t="s">
@@ -2906,9 +2889,6 @@
       <c r="S7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="8" spans="1:24" ht="75">
       <c r="A8" s="1" t="s">
@@ -2926,9 +2906,6 @@
       <c r="S8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="1" t="s">
@@ -2943,9 +2920,6 @@
       <c r="S9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="1" t="s">
@@ -2960,9 +2934,6 @@
       <c r="S10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V10" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
@@ -2977,9 +2948,6 @@
       <c r="S11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V11" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="1" t="s">
@@ -2994,9 +2962,6 @@
       <c r="S12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="13" spans="1:24" ht="105">
       <c r="A13" s="1" t="s">
@@ -3014,9 +2979,6 @@
       <c r="S13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="14" spans="1:24" ht="315">
       <c r="A14" s="1" t="s">
@@ -3037,9 +2999,6 @@
       <c r="U14" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="V14" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="15" spans="1:24" ht="315">
       <c r="A15" s="1" t="s">
@@ -3060,9 +3019,6 @@
       <c r="U15" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="V15" s="1" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="1" t="s">
@@ -3077,11 +3033,8 @@
       <c r="S16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
         <v>286</v>
       </c>
@@ -3094,11 +3047,8 @@
       <c r="S17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V17" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -3111,11 +3061,8 @@
       <c r="S18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V18" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="1" t="s">
         <v>293</v>
       </c>
@@ -3128,11 +3075,8 @@
       <c r="S19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V19" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="1" t="s">
         <v>296</v>
       </c>
@@ -3148,11 +3092,8 @@
       <c r="U20" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="V20" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>195</v>
       </c>
@@ -3165,11 +3106,8 @@
       <c r="S21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V21" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="90">
+    </row>
+    <row r="22" spans="1:21" ht="90">
       <c r="A22" t="s">
         <v>508</v>
       </c>
@@ -3186,13 +3124,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:21">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:21">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:21">
       <c r="A25"/>
     </row>
     <row r="56" spans="20:23" ht="18">
@@ -3204,7 +3142,7 @@
       <c r="W59" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3218,7 +3156,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3276,10 +3214,10 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3360,7 +3298,7 @@
         <v>432</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="75">
@@ -3988,7 +3926,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4053,10 +3991,10 @@
   <dimension ref="A1:AB95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AA65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA80" sqref="AA80"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
@@ -4359,9 +4297,6 @@
       <c r="K5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M5" s="1" t="s">
         <v>62</v>
       </c>
@@ -4619,9 +4554,6 @@
       </c>
       <c r="K10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>62</v>
@@ -4782,9 +4714,6 @@
       <c r="K13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M13" s="1" t="s">
         <v>62</v>
       </c>
@@ -5053,9 +4982,6 @@
       </c>
       <c r="K18" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>62</v>
@@ -5994,9 +5920,6 @@
       <c r="K37" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M37" s="1" t="s">
         <v>62</v>
       </c>
@@ -6266,9 +6189,6 @@
       <c r="K42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M42" s="1" t="s">
         <v>62</v>
       </c>
@@ -6585,9 +6505,6 @@
       <c r="K48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M48" s="1" t="s">
         <v>62</v>
       </c>
@@ -6851,9 +6768,6 @@
       <c r="K53" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M53" s="1" t="s">
         <v>62</v>
       </c>
@@ -7070,9 +6984,6 @@
       <c r="K57" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M57" s="1" t="s">
         <v>62</v>
       </c>
@@ -7282,9 +7193,6 @@
       <c r="K61" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L61" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M61" s="1" t="s">
         <v>62</v>
       </c>
@@ -7450,9 +7358,6 @@
       <c r="K64" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L64" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M64" s="1" t="s">
         <v>62</v>
       </c>
@@ -7822,9 +7727,6 @@
       <c r="K71" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M71" s="1" t="s">
         <v>62</v>
       </c>
@@ -8035,9 +7937,6 @@
       <c r="K75" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L75" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M75" s="1" t="s">
         <v>62</v>
       </c>
@@ -8150,9 +8049,6 @@
       <c r="K77" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M77" s="1" t="s">
         <v>62</v>
       </c>
@@ -8265,9 +8161,6 @@
       <c r="K79" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="M79" s="1" t="s">
         <v>62</v>
       </c>
@@ -9105,12 +8998,14 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="18.95" customHeight="1">
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
       <c r="Y95" s="5"/>
+      <c r="Z95" s="7"/>
+      <c r="AA95" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB94" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState ref="A7:AA34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9124,10 +9019,10 @@
   <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A87" sqref="A87"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
healthedata1 Preapply GF#23925, GF#23923
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-server.xlsx
+++ b/source/source_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215D7201-681F-4B77-988E-50559920204C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4071D91A-ED36-49C3-90A5-D9FFFA500783}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="523">
   <si>
     <t>Element</t>
   </si>
@@ -1730,6 +1730,9 @@
   </si>
   <si>
     <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;authoredon=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;authoredon=ge2019&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>!PractitionerRole</t>
   </si>
 </sst>
 </file>
@@ -4117,11 +4120,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AB38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="AB68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomRight" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
@@ -9014,7 +9017,7 @@
         <v>89</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>296</v>
+        <v>522</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>297</v>
@@ -9027,7 +9030,7 @@
       </c>
       <c r="F93" s="1" t="str">
         <f t="shared" si="29"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!practitionerrole</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>62</v>
@@ -9040,7 +9043,7 @@
       </c>
       <c r="J93" s="1" t="str">
         <f t="shared" si="37"/>
-        <v>PractitionerRole.specialty</v>
+        <v>!PractitionerRole.specialty</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>62</v>
@@ -9059,11 +9062,11 @@
       </c>
       <c r="AA93" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B93&amp;" resources matching the specialty"</f>
-        <v>Fetches a bundle containing  PractitionerRole resources matching the specialty</v>
+        <v>Fetches a bundle containing  !PractitionerRole resources matching the specialty</v>
       </c>
       <c r="AB93" s="1" t="str">
         <f t="shared" ref="AB93" si="41">"SearchParameter-us-core-"&amp;LOWER((B93)&amp;"-"&amp;SUBSTITUTE(C93,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
+        <v>SearchParameter-us-core-!practitionerrole-specialty.html</v>
       </c>
     </row>
     <row r="94" spans="1:28" ht="18.95" customHeight="1">
@@ -9071,7 +9074,7 @@
         <v>90</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>296</v>
+        <v>522</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>298</v>
@@ -9084,7 +9087,7 @@
       </c>
       <c r="F94" s="1" t="str">
         <f t="shared" si="29"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!practitionerrole</v>
       </c>
       <c r="G94" t="s">
         <v>62</v>
@@ -9097,7 +9100,7 @@
       </c>
       <c r="J94" s="1" t="str">
         <f t="shared" si="37"/>
-        <v>PractitionerRole.practitioner</v>
+        <v>!PractitionerRole.practitioner</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>62</v>
@@ -9119,11 +9122,11 @@
       </c>
       <c r="AA94" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B94&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
-        <v>Fetches a bundle containing  PractitionerRole resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint.</v>
+        <v>Fetches a bundle containing  !PractitionerRole resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint.</v>
       </c>
       <c r="AB94" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B94)&amp;"-"&amp;SUBSTITUTE(C94,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
+        <v>SearchParameter-us-core-!practitionerrole-practitioner.html</v>
       </c>
     </row>
   </sheetData>
@@ -9141,8 +9144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>